<commit_message>
Replacing missing values using mode
</commit_message>
<xml_diff>
--- a/dataset1.xlsx
+++ b/dataset1.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1467" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1456" uniqueCount="13">
   <si>
     <t>type</t>
   </si>
@@ -356,7 +356,7 @@
   <dimension ref="A1:E1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H75" sqref="H75"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -400,9 +400,7 @@
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>5</v>
-      </c>
+      <c r="B3" s="2"/>
       <c r="C3" s="3" t="s">
         <v>6</v>
       </c>
@@ -429,9 +427,7 @@
       <c r="B5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>6</v>
-      </c>
+      <c r="C5" s="3"/>
       <c r="D5" s="2">
         <v>4</v>
       </c>
@@ -440,9 +436,7 @@
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>5</v>
-      </c>
+      <c r="B6" s="2"/>
       <c r="C6" s="3" t="s">
         <v>6</v>
       </c>
@@ -468,9 +462,7 @@
       <c r="A8" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>5</v>
-      </c>
+      <c r="B8" s="2"/>
       <c r="C8" s="3" t="s">
         <v>6</v>
       </c>
@@ -876,9 +868,7 @@
       <c r="A38" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B38" s="2" t="s">
-        <v>5</v>
-      </c>
+      <c r="B38" s="2"/>
       <c r="C38" s="3" t="s">
         <v>6</v>
       </c>
@@ -890,9 +880,7 @@
       <c r="A39" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B39" s="2" t="s">
-        <v>5</v>
-      </c>
+      <c r="B39" s="2"/>
       <c r="C39" s="3" t="s">
         <v>6</v>
       </c>
@@ -904,9 +892,7 @@
       <c r="A40" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B40" s="2" t="s">
-        <v>5</v>
-      </c>
+      <c r="B40" s="2"/>
       <c r="C40" s="3" t="s">
         <v>6</v>
       </c>
@@ -918,9 +904,7 @@
       <c r="A41" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B41" s="2" t="s">
-        <v>5</v>
-      </c>
+      <c r="B41" s="2"/>
       <c r="C41" s="3" t="s">
         <v>6</v>
       </c>
@@ -932,9 +916,7 @@
       <c r="A42" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B42" s="2" t="s">
-        <v>5</v>
-      </c>
+      <c r="B42" s="2"/>
       <c r="C42" s="3" t="s">
         <v>6</v>
       </c>
@@ -946,9 +928,7 @@
       <c r="A43" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B43" s="2" t="s">
-        <v>5</v>
-      </c>
+      <c r="B43" s="2"/>
       <c r="C43" s="3" t="s">
         <v>6</v>
       </c>
@@ -960,9 +940,7 @@
       <c r="A44" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B44" s="2" t="s">
-        <v>5</v>
-      </c>
+      <c r="B44" s="2"/>
       <c r="C44" s="3" t="s">
         <v>6</v>
       </c>
@@ -2066,9 +2044,7 @@
       <c r="C123" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D123" s="2">
-        <v>4</v>
-      </c>
+      <c r="D123" s="2"/>
     </row>
     <row r="124" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A124" s="2" t="s">
@@ -2080,9 +2056,7 @@
       <c r="C124" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D124" s="2">
-        <v>4</v>
-      </c>
+      <c r="D124" s="2"/>
     </row>
     <row r="125" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A125" s="2" t="s">
@@ -2094,9 +2068,7 @@
       <c r="C125" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D125" s="2">
-        <v>4</v>
-      </c>
+      <c r="D125" s="2"/>
     </row>
     <row r="126" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A126" s="2" t="s">
@@ -2108,9 +2080,7 @@
       <c r="C126" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D126" s="2">
-        <v>4</v>
-      </c>
+      <c r="D126" s="2"/>
     </row>
     <row r="127" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A127" s="2" t="s">
@@ -2122,9 +2092,7 @@
       <c r="C127" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D127" s="2">
-        <v>4</v>
-      </c>
+      <c r="D127" s="2"/>
     </row>
     <row r="128" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A128" s="2" t="s">
@@ -2136,9 +2104,7 @@
       <c r="C128" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D128" s="2">
-        <v>4</v>
-      </c>
+      <c r="D128" s="2"/>
     </row>
     <row r="129" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A129" s="2" t="s">
@@ -2150,9 +2116,7 @@
       <c r="C129" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D129" s="2">
-        <v>4</v>
-      </c>
+      <c r="D129" s="2"/>
     </row>
     <row r="130" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A130" s="2" t="s">

</xml_diff>